<commit_message>
changes in ui All Images Removed
</commit_message>
<xml_diff>
--- a/FinalUi/Data/VORTEX_ALPHA_TEST_REPORT.xlsx
+++ b/FinalUi/Data/VORTEX_ALPHA_TEST_REPORT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pankaj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pankaj\Documents\billingsystem\FinalUi\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PROBLEMS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
   <si>
     <t xml:space="preserve">TITLE </t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>resolved</t>
+  </si>
+  <si>
+    <t>ved</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -1262,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,6 +1294,9 @@
       <c r="A4" t="s">
         <v>65</v>
       </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>